<commit_message>
updated syllabus student engagement
</commit_message>
<xml_diff>
--- a/data/syllabus645.xlsx
+++ b/data/syllabus645.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conglizhang/Documents/0_0_projects/EDUC-quant-sequence/645/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markhammond/Documents/GitHub/645/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB4DBD1-424B-8547-AEF2-C579057ECA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E93465-D3EE-D74C-8183-0FFFC4DD2E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="680" windowWidth="21340" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38640" yWindow="2260" windowWidth="28560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Units</t>
   </si>
@@ -244,7 +244,34 @@
     <t>Missing Data</t>
   </si>
   <si>
-    <t>Uniti Topics</t>
+    <t>Unit Topics</t>
+  </si>
+  <si>
+    <t>Recommended Readings</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 2 (pp. xx-xx), 6-6.4 (pp. xx-xx)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 9-9.7 (pp. xx-xx)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 7-7.8 (pp. xx-xx)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 8.6-8.11 (pp. xx-xx)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 8-8.5 (pp. xx-xx)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 4.5-4.10 (pp. xx-xx) Ch. 5 (pp. xx-xx)</t>
+  </si>
+  <si>
+    <t>BMLR Ch.4-4.4 (pp. xx-xx)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 6.5-6.7 (pp. xx-xx)</t>
   </si>
 </sst>
 </file>
@@ -288,13 +315,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -577,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E022E340-D6CD-FB4A-97CB-6547073D4063}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -591,12 +618,13 @@
     <col min="4" max="4" width="35.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="17" style="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,13 +644,16 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -639,8 +670,9 @@
         <v>45</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
         <v>24</v>
@@ -648,11 +680,14 @@
       <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
@@ -662,11 +697,14 @@
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
         <v>27</v>
@@ -674,9 +712,10 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
@@ -688,9 +727,10 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
         <v>29</v>
@@ -699,14 +739,15 @@
         <v>31</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -722,9 +763,12 @@
       <c r="E8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>43</v>
@@ -733,8 +777,9 @@
         <v>46</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -744,9 +789,12 @@
       <c r="E10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
         <v>48</v>
@@ -755,14 +803,15 @@
         <v>50</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -778,11 +827,14 @@
       <c r="E12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="2"/>
       <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
         <v>52</v>
@@ -791,8 +843,9 @@
         <v>53</v>
       </c>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
@@ -800,17 +853,21 @@
       <c r="E14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3" t="s">
         <v>56</v>
       </c>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -818,23 +875,27 @@
       <c r="E16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2"/>
+      <c r="H17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -848,33 +909,38 @@
       <c r="E18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3" t="s">
         <v>61</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2"/>
+      <c r="H20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -891,24 +957,26 @@
         <v>22</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2"/>
+      <c r="H22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
@@ -918,20 +986,22 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="2"/>
+      <c r="H23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C25" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating final & datasets
</commit_message>
<xml_diff>
--- a/data/syllabus645.xlsx
+++ b/data/syllabus645.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markhammond/Documents/GitHub/645/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conglizhang/Documents/0_0_projects/EDUC-quant-sequence/645/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF73417-48D5-684D-8348-604A13D6903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF19456F-95B6-CA45-9D64-F31C1274F23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21340" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21340" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>a. Logistic regression programming in R</t>
   </si>
   <si>
-    <t>a. Review Unit 4 assignment/quiz</t>
-  </si>
-  <si>
     <t xml:space="preserve">a. Review OLS
 </t>
   </si>
@@ -124,9 +121,6 @@
 </t>
   </si>
   <si>
-    <t>b. Preview Unit 1 assignment/quiz</t>
-  </si>
-  <si>
     <t>Assignment 1 (Due: TBD)</t>
   </si>
   <si>
@@ -164,10 +158,6 @@
     <t>b. Poisson regression analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">a. Review Unit 1 assignment/quiz
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">a. R basics and R packages
 </t>
   </si>
@@ -186,9 +176,6 @@
 </t>
   </si>
   <si>
-    <t>b. Preview Unit 2 assignment/quiz</t>
-  </si>
-  <si>
     <t xml:space="preserve">a. Clustering within datasets
 </t>
   </si>
@@ -199,33 +186,17 @@
     <t>b. Visualize/understand nested data</t>
   </si>
   <si>
-    <t>a. Review Unit 2 assignment/quiz</t>
-  </si>
-  <si>
     <t xml:space="preserve">a. Nested data and OLS estimator
 </t>
   </si>
   <si>
-    <t>b. Preview Unit 3 assignment/quiz</t>
-  </si>
-  <si>
-    <t>b. Preview and prepare for final project</t>
-  </si>
-  <si>
     <t>a. Nested data and Logistic regression</t>
   </si>
   <si>
-    <t xml:space="preserve">a. Review Unit 3 assignment/quiz
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">b. Measurement and assessment in R
 </t>
   </si>
   <si>
-    <t>c. Preview Unit 4 assignment/quiz</t>
-  </si>
-  <si>
     <t>b. Dealing with missing data in R</t>
   </si>
   <si>
@@ -275,6 +246,35 @@
   </si>
   <si>
     <t>BMLR 9-9.7 (pp. xx-xx), Ch 11</t>
+  </si>
+  <si>
+    <t>b. Preview Unit 1 assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. Review Unit 1 assignment
+</t>
+  </si>
+  <si>
+    <t>a. Review Unit 2 assignment</t>
+  </si>
+  <si>
+    <t>b. Preview Unit 3 assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. Review Unit 3 assignment
+</t>
+  </si>
+  <si>
+    <t>c. Preview Unit 4 assignment</t>
+  </si>
+  <si>
+    <t>a. Review Unit 4 assignment</t>
+  </si>
+  <si>
+    <t>b. Preview Unit 2 assignment and final project</t>
+  </si>
+  <si>
+    <t>b. Prepare for final project</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -647,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -661,31 +661,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -697,13 +697,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -712,7 +712,7 @@
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -725,10 +725,10 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -738,18 +738,18 @@
     <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -757,29 +757,29 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -789,31 +789,31 @@
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -821,19 +821,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="3"/>
@@ -842,10 +842,10 @@
     <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -856,10 +856,10 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -867,7 +867,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -878,10 +878,10 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -889,15 +889,15 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -905,17 +905,17 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="3" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="3"/>
@@ -925,7 +925,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -934,15 +934,15 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -950,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
@@ -959,7 +959,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -970,15 +970,15 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
syllabus and measure slides updates
</commit_message>
<xml_diff>
--- a/data/syllabus645.xlsx
+++ b/data/syllabus645.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markhammond/Documents/GitHub/645/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF73417-48D5-684D-8348-604A13D6903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BCBF35-3328-FE47-A80B-AA90F0AE7A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21340" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25540" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Units</t>
   </si>
@@ -250,9 +250,6 @@
     <t>Recommended Readings</t>
   </si>
   <si>
-    <t>BMLR 7-7.8 (pp. xx-xx)</t>
-  </si>
-  <si>
     <t>BMLR Ch. 2 (pp. xx-xx), 6-6.4 (pp. xx-xx)</t>
   </si>
   <si>
@@ -275,6 +272,12 @@
   </si>
   <si>
     <t>BMLR 9-9.7 (pp. xx-xx), Ch 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMLR 7-7.8 (pp. xx-xx); </t>
+  </si>
+  <si>
+    <t>IEPM Ch. 5 &amp; 6</t>
   </si>
 </sst>
 </file>
@@ -610,7 +613,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -673,10 +676,10 @@
         <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -703,7 +706,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -769,7 +772,7 @@
         <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -795,7 +798,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -833,7 +836,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="3"/>
@@ -859,7 +862,7 @@
         <v>55</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -881,7 +884,7 @@
         <v>58</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -915,7 +918,7 @@
         <v>59</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="3"/>
@@ -927,7 +930,9 @@
       <c r="E19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updates to syllabus learning objectives
</commit_message>
<xml_diff>
--- a/data/syllabus645.xlsx
+++ b/data/syllabus645.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markhammond/Documents/GitHub/645/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BCBF35-3328-FE47-A80B-AA90F0AE7A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94DD9FC-C306-984A-94CD-210D7B85D6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25540" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,34 +250,34 @@
     <t>Recommended Readings</t>
   </si>
   <si>
-    <t>BMLR Ch. 2 (pp. xx-xx), 6-6.4 (pp. xx-xx)</t>
-  </si>
-  <si>
-    <t>BMLR 3.3 'Discrete Random Variables' (pp. xx-xx)</t>
-  </si>
-  <si>
-    <t>BMLR 6.5-6.7 (pp. xx-xx)</t>
-  </si>
-  <si>
-    <t>BMLR  4-4.4 (pp. xx-xx)</t>
-  </si>
-  <si>
-    <t>BMLR  4.5-4.10 (pp. xx-xx), Ch. 5 (pp. xx-xx)</t>
-  </si>
-  <si>
-    <t>BMLR 8-8.5 (pp. xx-xx)</t>
-  </si>
-  <si>
-    <t>BMLR 8.6-8.11 (pp. xx-xx)</t>
-  </si>
-  <si>
-    <t>BMLR 9-9.7 (pp. xx-xx), Ch 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMLR 7-7.8 (pp. xx-xx); </t>
-  </si>
-  <si>
     <t>IEPM Ch. 5 &amp; 6</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 2 (pp. 39-68), 6.1-6.4 (pp. 151-155)</t>
+  </si>
+  <si>
+    <t>BMLR 3.3 'Discrete Random Variables' (pp. 72-79)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 6.5-6.7 (pp. 159-180)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 4.1-4.4 (pp. 93-112)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 4.5-4.10 (pp. 113-132), Ch. 5 (pp. 145-148)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 8.1-8.5 (pp. 211-231)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 8.6-8.11 (pp. 234-251)</t>
+  </si>
+  <si>
+    <t>BMLR Ch. 9.1-9.7 (pp. 263-306), Ch. 11 (pp. 373-398)</t>
+  </si>
+  <si>
+    <t>BMLR 7.1-7.8 (pp. 193-206)</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E022E340-D6CD-FB4A-97CB-6547073D4063}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -676,10 +676,10 @@
         <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -706,7 +706,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -772,7 +772,7 @@
         <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -798,7 +798,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -836,7 +836,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="3"/>
@@ -862,7 +862,7 @@
         <v>55</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -884,7 +884,7 @@
         <v>58</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -918,7 +918,7 @@
         <v>59</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="3"/>
@@ -931,7 +931,7 @@
         <v>60</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G19" s="2"/>
     </row>

</xml_diff>

<commit_message>
minor updates and new principal data
</commit_message>
<xml_diff>
--- a/data/syllabus645.xlsx
+++ b/data/syllabus645.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markhammond/Documents/GitHub/645/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D1AA74-1F12-A34F-A093-E29A3C4131C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F68A448-F2A5-1E48-A40C-3B7DDC392116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="21600" windowHeight="25620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="-2020" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -604,9 +604,9 @@
     <col min="1" max="1" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="17" style="1"/>
   </cols>
@@ -713,7 +713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
         <v>19</v>
@@ -819,7 +819,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>